<commit_message>
modified home/存股/自己存股-每年複利計算.xlsx at 2018/04/10 20:22
</commit_message>
<xml_diff>
--- a/home/存股/自己存股-每年複利計算.xlsx
+++ b/home/存股/自己存股-每年複利計算.xlsx
@@ -370,7 +370,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -381,7 +381,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -438,7 +438,7 @@
         <v>654539.10600000003</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B16" si="0">F3-A3</f>
+        <f t="shared" ref="B3:B21" si="0">F3-A3</f>
         <v>627820.89399999997</v>
       </c>
       <c r="C3" s="1">
@@ -773,99 +773,119 @@
         <f t="shared" si="2"/>
         <v>7800000</v>
       </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>200000</v>
+      </c>
       <c r="C17" s="1">
         <v>0.04</v>
       </c>
       <c r="D17">
         <f t="shared" si="3"/>
-        <v>312000</v>
+        <v>320000</v>
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
-        <v>8112000</v>
+        <v>8320000</v>
       </c>
       <c r="F17">
-        <v>7500000</v>
+        <v>8000000</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18">
         <f t="shared" si="2"/>
-        <v>8112000</v>
+        <v>8320000</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>180000</v>
       </c>
       <c r="C18" s="1">
         <v>0.04</v>
       </c>
       <c r="D18">
         <f t="shared" si="3"/>
-        <v>324480</v>
+        <v>340000</v>
       </c>
       <c r="E18">
         <f t="shared" si="1"/>
-        <v>8436480</v>
+        <v>8840000</v>
       </c>
       <c r="F18">
-        <v>8000000</v>
+        <v>8500000</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19">
         <f t="shared" si="2"/>
-        <v>8436480</v>
+        <v>8840000</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>160000</v>
       </c>
       <c r="C19" s="1">
         <v>0.04</v>
       </c>
       <c r="D19">
         <f t="shared" si="3"/>
-        <v>337459.20000000001</v>
+        <v>360000</v>
       </c>
       <c r="E19">
         <f t="shared" si="1"/>
-        <v>8773939.1999999993</v>
+        <v>9360000</v>
       </c>
       <c r="F19">
-        <v>8500000</v>
+        <v>9000000</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20">
         <f t="shared" si="2"/>
-        <v>8773939.1999999993</v>
+        <v>9360000</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>140000</v>
       </c>
       <c r="C20" s="1">
         <v>0.04</v>
       </c>
       <c r="D20">
         <f t="shared" si="3"/>
-        <v>350957.56799999997</v>
+        <v>380000</v>
       </c>
       <c r="E20">
         <f t="shared" si="1"/>
-        <v>9124896.7679999992</v>
+        <v>9880000</v>
       </c>
       <c r="F20">
-        <v>9000000</v>
+        <v>9500000</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21">
         <f t="shared" si="2"/>
-        <v>9124896.7679999992</v>
+        <v>9880000</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>120000</v>
       </c>
       <c r="C21" s="1">
         <v>0.04</v>
       </c>
       <c r="D21">
         <f t="shared" si="3"/>
-        <v>364995.87071999995</v>
+        <v>400000</v>
       </c>
       <c r="E21">
         <f t="shared" si="1"/>
-        <v>9489892.6387199983</v>
+        <v>10400000</v>
       </c>
       <c r="F21">
-        <v>9500000</v>
+        <v>10000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified home/存股/... at 2018/04/25
</commit_message>
<xml_diff>
--- a/home/存股/自己存股-每年複利計算.xlsx
+++ b/home/存股/自己存股-每年複利計算.xlsx
@@ -381,7 +381,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -392,7 +392,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -453,15 +453,15 @@
         <v>615602.89399999997</v>
       </c>
       <c r="C3" s="3">
-        <v>5.1999999999999998E-2</v>
+        <v>5.3100000000000001E-2</v>
       </c>
       <c r="D3">
         <f>(A3+B3)*C3</f>
-        <v>66047.383999999991</v>
+        <v>67444.540200000003</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E21" si="1">A3+B3+D3</f>
-        <v>1336189.3840000001</v>
+        <v>1337586.5401999999</v>
       </c>
       <c r="F3" s="2">
         <v>1270142</v>
@@ -470,11 +470,11 @@
     <row r="4" spans="1:6">
       <c r="A4">
         <f t="shared" ref="A4:A21" si="2">E3</f>
-        <v>1336189.3840000001</v>
+        <v>1337586.5401999999</v>
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>163810.61599999992</v>
+        <v>162413.45980000007</v>
       </c>
       <c r="C4" s="1">
         <v>0.04</v>

</xml_diff>

<commit_message>
modified home/存股/... at 2018/04/26
</commit_message>
<xml_diff>
--- a/home/存股/自己存股-每年複利計算.xlsx
+++ b/home/存股/自己存股-每年複利計算.xlsx
@@ -381,7 +381,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -392,7 +392,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -450,31 +450,31 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B21" si="0">F3-A3</f>
-        <v>615602.89399999997</v>
+        <v>637486.89399999997</v>
       </c>
       <c r="C3" s="3">
-        <v>5.3100000000000001E-2</v>
+        <v>5.2900000000000003E-2</v>
       </c>
       <c r="D3">
         <f>(A3+B3)*C3</f>
-        <v>67444.540200000003</v>
+        <v>68348.175400000007</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E21" si="1">A3+B3+D3</f>
-        <v>1337586.5401999999</v>
+        <v>1360374.1754000001</v>
       </c>
       <c r="F3" s="2">
-        <v>1270142</v>
+        <v>1292026</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
         <f t="shared" ref="A4:A21" si="2">E3</f>
-        <v>1337586.5401999999</v>
+        <v>1360374.1754000001</v>
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>162413.45980000007</v>
+        <v>139625.82459999993</v>
       </c>
       <c r="C4" s="1">
         <v>0.04</v>

</xml_diff>

<commit_message>
modifed home/存股/... at 2018/05/15
</commit_message>
<xml_diff>
--- a/home/存股/自己存股-每年複利計算.xlsx
+++ b/home/存股/自己存股-每年複利計算.xlsx
@@ -380,7 +380,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -391,7 +391,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -447,43 +447,43 @@
         <f>E2</f>
         <v>654539.10600000003</v>
       </c>
-      <c r="B3">
-        <f t="shared" ref="B3:B21" si="0">F3-A3</f>
-        <v>637486.89399999997</v>
+      <c r="B3" s="2">
+        <f>F3-A3</f>
+        <v>680616.89399999997</v>
       </c>
       <c r="C3" s="3">
-        <v>5.3100000000000001E-2</v>
+        <v>5.3199999999999997E-2</v>
       </c>
       <c r="D3">
         <f>(A3+B3)*C3</f>
-        <v>68606.580600000001</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E21" si="1">A3+B3+D3</f>
-        <v>1360632.5806</v>
+        <v>71030.299199999994</v>
+      </c>
+      <c r="E3" s="2">
+        <f>A3+B3+D3</f>
+        <v>1406186.2992</v>
       </c>
       <c r="F3" s="2">
-        <v>1292026</v>
+        <v>1335156</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <f t="shared" ref="A4:A21" si="2">E3</f>
-        <v>1360632.5806</v>
+        <f>E3</f>
+        <v>1406186.2992</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
-        <v>139367.41940000001</v>
+        <f t="shared" ref="B3:B21" si="0">F4-A4</f>
+        <v>93813.700799999991</v>
       </c>
       <c r="C4" s="1">
         <v>0.04</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D21" si="3">(A4+B4)*C4</f>
+        <f t="shared" ref="D4:D21" si="1">(A4+B4)*C4</f>
         <v>60000</v>
       </c>
       <c r="E4">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="E3:E21" si="2">A4+B4+D4</f>
         <v>1560000</v>
       </c>
       <c r="F4">
@@ -492,7 +492,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="A4:A21" si="3">E4</f>
         <v>1560000</v>
       </c>
       <c r="B5">
@@ -503,11 +503,11 @@
         <v>0.04</v>
       </c>
       <c r="D5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>80000</v>
       </c>
       <c r="E5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2080000</v>
       </c>
       <c r="F5">
@@ -516,7 +516,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2080000</v>
       </c>
       <c r="B6">
@@ -527,11 +527,11 @@
         <v>0.04</v>
       </c>
       <c r="D6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>100000</v>
       </c>
       <c r="E6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2600000</v>
       </c>
       <c r="F6">
@@ -540,7 +540,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2600000</v>
       </c>
       <c r="B7">
@@ -551,11 +551,11 @@
         <v>0.04</v>
       </c>
       <c r="D7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>120000</v>
       </c>
       <c r="E7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3120000</v>
       </c>
       <c r="F7">
@@ -564,7 +564,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3120000</v>
       </c>
       <c r="B8">
@@ -575,11 +575,11 @@
         <v>0.04</v>
       </c>
       <c r="D8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>140000</v>
       </c>
       <c r="E8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3640000</v>
       </c>
       <c r="F8">
@@ -588,7 +588,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3640000</v>
       </c>
       <c r="B9">
@@ -599,11 +599,11 @@
         <v>0.04</v>
       </c>
       <c r="D9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>160000</v>
       </c>
       <c r="E9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4160000</v>
       </c>
       <c r="F9">
@@ -612,7 +612,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4160000</v>
       </c>
       <c r="B10">
@@ -623,11 +623,11 @@
         <v>0.04</v>
       </c>
       <c r="D10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>180000</v>
       </c>
       <c r="E10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4680000</v>
       </c>
       <c r="F10">
@@ -636,7 +636,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4680000</v>
       </c>
       <c r="B11">
@@ -647,11 +647,11 @@
         <v>0.04</v>
       </c>
       <c r="D11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>200000</v>
       </c>
       <c r="E11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5200000</v>
       </c>
       <c r="F11">
@@ -660,7 +660,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5200000</v>
       </c>
       <c r="B12">
@@ -671,11 +671,11 @@
         <v>0.04</v>
       </c>
       <c r="D12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>220000</v>
       </c>
       <c r="E12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5720000</v>
       </c>
       <c r="F12">
@@ -684,7 +684,7 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5720000</v>
       </c>
       <c r="B13">
@@ -695,11 +695,11 @@
         <v>0.04</v>
       </c>
       <c r="D13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>240000</v>
       </c>
       <c r="E13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6240000</v>
       </c>
       <c r="F13">
@@ -708,7 +708,7 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6240000</v>
       </c>
       <c r="B14">
@@ -719,11 +719,11 @@
         <v>0.04</v>
       </c>
       <c r="D14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>260000</v>
       </c>
       <c r="E14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6760000</v>
       </c>
       <c r="F14">
@@ -732,7 +732,7 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6760000</v>
       </c>
       <c r="B15">
@@ -743,11 +743,11 @@
         <v>0.04</v>
       </c>
       <c r="D15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>280000</v>
       </c>
       <c r="E15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7280000</v>
       </c>
       <c r="F15">
@@ -756,7 +756,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7280000</v>
       </c>
       <c r="B16">
@@ -767,11 +767,11 @@
         <v>0.04</v>
       </c>
       <c r="D16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>300000</v>
       </c>
       <c r="E16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7800000</v>
       </c>
       <c r="F16">
@@ -780,7 +780,7 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7800000</v>
       </c>
       <c r="B17">
@@ -791,11 +791,11 @@
         <v>0.04</v>
       </c>
       <c r="D17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>320000</v>
       </c>
       <c r="E17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8320000</v>
       </c>
       <c r="F17">
@@ -804,7 +804,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8320000</v>
       </c>
       <c r="B18">
@@ -815,11 +815,11 @@
         <v>0.04</v>
       </c>
       <c r="D18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>340000</v>
       </c>
       <c r="E18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8840000</v>
       </c>
       <c r="F18">
@@ -828,7 +828,7 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8840000</v>
       </c>
       <c r="B19">
@@ -839,11 +839,11 @@
         <v>0.04</v>
       </c>
       <c r="D19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>360000</v>
       </c>
       <c r="E19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9360000</v>
       </c>
       <c r="F19">
@@ -852,7 +852,7 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9360000</v>
       </c>
       <c r="B20">
@@ -863,11 +863,11 @@
         <v>0.04</v>
       </c>
       <c r="D20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>380000</v>
       </c>
       <c r="E20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9880000</v>
       </c>
       <c r="F20">
@@ -876,7 +876,7 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9880000</v>
       </c>
       <c r="B21">
@@ -887,11 +887,11 @@
         <v>0.04</v>
       </c>
       <c r="D21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>400000</v>
       </c>
       <c r="E21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10400000</v>
       </c>
       <c r="F21">

</xml_diff>